<commit_message>
CS Test - Modificaiton
</commit_message>
<xml_diff>
--- a/properties/env/qa/data/Trade_Data.xlsx
+++ b/properties/env/qa/data/Trade_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ptuptewar\Repo\WebTAF\properties\env\qa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12646E11-FC02-4C49-8783-1615C08ED3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49561CBF-3CD5-496E-9EB4-201B4448B627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario_1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="17">
   <si>
     <t>TC_Name</t>
   </si>
@@ -89,7 +89,52 @@
     <t>{
     "customer": "PLUTO1",
     "ccyPair": "EURUSD",
-    "type": "Spot",
+    "type": "$type",
+    "direction": "BUY",
+    "tradeDate": "$tradeDate",
+    "amount1": 1000000.00,
+    "amount2": 1120000.00,
+    "rate": 1.12,
+    "valueDate": "$valueDate",
+    "legalEntity": "CS, Zurich",
+    "trader": "Johann Baumfiddler"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "customer": "PLUTO1",
+    "ccyPair": "INRUSD",
+    "type": "$type",
+    "direction": "BUY",
+    "tradeDate": "$tradeDate",
+    "amount1": 1000000.00,
+    "amount2": 1120000.00,
+    "rate": 1.12,
+    "valueDate": "$valueDate",
+    "legalEntity": "$legalEntity",
+    "trader": "Johann Baumfiddler"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "customer": "PLUTO1",
+    "ccyPair": "INRUSD",
+    "type": "$type",
+    "direction": "BUY",
+    "tradeDate": "$tradeDate",
+    "amount1": 1000000.00,
+    "amount2": 1120000.00,
+    "rate": 1.12,
+    "valueDate": "$valueDate",
+    "legalEntity": $legalEntity",
+    "trader": "Johann Baumfiddler"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "customer": "PLUTO1",
+    "ccyPair": "$ccyPair",
+    "type": "$type",
     "direction": "BUY",
     "tradeDate": "$tradeDate",
     "amount1": 1000000.00,
@@ -454,7 +499,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -504,7 +549,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -530,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90CDDF84-DB62-4619-9E29-8DBE75A5523A}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -581,7 +626,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -608,7 +653,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -658,7 +703,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -685,7 +730,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -735,7 +780,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -838,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8C0DF8-C161-4CD9-A6DA-7819C269548E}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -889,7 +934,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>